<commit_message>
1. GPS monitor locationForm 2. Legend. (remove maintain) 3. History report default start 4. wording 5. Fix over law standard bug
</commit_message>
<xml_diff>
--- a/report_template/all_daily_report.xlsx
+++ b/report_template/all_daily_report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
   <si>
     <t>監測日報表</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>維修</t>
-  </si>
-  <si>
-    <t>定保</t>
   </si>
   <si>
     <t>異常</t>
@@ -262,7 +259,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,12 +280,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -300,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -343,6 +334,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -380,13 +397,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -421,6 +432,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6575,7 +6592,7 @@
   <dimension ref="A1:AO40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -6589,40 +6606,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -6634,42 +6651,42 @@
       <c r="AO1" s="1"/>
     </row>
     <row r="2" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF2" s="20"/>
+      <c r="A2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF2" s="18"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
@@ -6681,34 +6698,32 @@
       <c r="AO2" s="1"/>
     </row>
     <row r="3" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" s="23"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="21"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -6738,10 +6753,10 @@
         <v>6</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>7</v>
@@ -6750,52 +6765,52 @@
         <v>8</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="W4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="Y4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>10</v>
@@ -10499,40 +10514,40 @@
       <c r="AO35" s="1"/>
     </row>
     <row r="36" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
-      <c r="T36" s="17"/>
-      <c r="U36" s="17"/>
-      <c r="V36" s="17"/>
-      <c r="W36" s="17"/>
-      <c r="X36" s="17"/>
-      <c r="Y36" s="17"/>
-      <c r="Z36" s="17"/>
-      <c r="AA36" s="17"/>
-      <c r="AB36" s="17"/>
-      <c r="AC36" s="17"/>
-      <c r="AD36" s="17"/>
-      <c r="AE36" s="17"/>
-      <c r="AF36" s="17"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="15"/>
+      <c r="AF36" s="15"/>
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
@@ -10544,38 +10559,38 @@
       <c r="AO36" s="1"/>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
-      <c r="T37" s="17"/>
-      <c r="U37" s="17"/>
-      <c r="V37" s="17"/>
-      <c r="W37" s="17"/>
-      <c r="X37" s="17"/>
-      <c r="Y37" s="17"/>
-      <c r="Z37" s="17"/>
-      <c r="AA37" s="17"/>
-      <c r="AB37" s="17"/>
-      <c r="AC37" s="17"/>
-      <c r="AD37" s="17"/>
-      <c r="AE37" s="17"/>
-      <c r="AF37" s="17"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="15"/>
+      <c r="AF37" s="15"/>
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
@@ -10587,38 +10602,38 @@
       <c r="AO37" s="1"/>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
-      <c r="T38" s="17"/>
-      <c r="U38" s="17"/>
-      <c r="V38" s="17"/>
-      <c r="W38" s="17"/>
-      <c r="X38" s="17"/>
-      <c r="Y38" s="17"/>
-      <c r="Z38" s="17"/>
-      <c r="AA38" s="17"/>
-      <c r="AB38" s="17"/>
-      <c r="AC38" s="17"/>
-      <c r="AD38" s="17"/>
-      <c r="AE38" s="17"/>
-      <c r="AF38" s="17"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="15"/>
+      <c r="AF38" s="15"/>
       <c r="AG38" s="1"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
@@ -10630,38 +10645,38 @@
       <c r="AO38" s="1"/>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
-      <c r="T39" s="17"/>
-      <c r="U39" s="17"/>
-      <c r="V39" s="17"/>
-      <c r="W39" s="17"/>
-      <c r="X39" s="17"/>
-      <c r="Y39" s="17"/>
-      <c r="Z39" s="17"/>
-      <c r="AA39" s="17"/>
-      <c r="AB39" s="17"/>
-      <c r="AC39" s="17"/>
-      <c r="AD39" s="17"/>
-      <c r="AE39" s="17"/>
-      <c r="AF39" s="17"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
+      <c r="V39" s="15"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+      <c r="AC39" s="15"/>
+      <c r="AD39" s="15"/>
+      <c r="AE39" s="15"/>
+      <c r="AF39" s="15"/>
       <c r="AG39" s="1"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
@@ -10673,38 +10688,38 @@
       <c r="AO39" s="1"/>
     </row>
     <row r="40" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
-      <c r="T40" s="17"/>
-      <c r="U40" s="17"/>
-      <c r="V40" s="17"/>
-      <c r="W40" s="17"/>
-      <c r="X40" s="17"/>
-      <c r="Y40" s="17"/>
-      <c r="Z40" s="17"/>
-      <c r="AA40" s="17"/>
-      <c r="AB40" s="17"/>
-      <c r="AC40" s="17"/>
-      <c r="AD40" s="17"/>
-      <c r="AE40" s="17"/>
-      <c r="AF40" s="17"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="15"/>
+      <c r="AF40" s="15"/>
       <c r="AG40" s="1"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
@@ -10716,7 +10731,7 @@
       <c r="AO40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="B36:AF40"/>
     <mergeCell ref="A1:AF1"/>
@@ -10724,6 +10739,7 @@
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>